<commit_message>
Delete Select Order By nr
</commit_message>
<xml_diff>
--- a/for-tests/FlightGUIBU/Default.xlsx
+++ b/for-tests/FlightGUIBU/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="14"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="Order By Ad" sheetId="9" r:id="rId9"/>
     <sheet name="New Search" sheetId="10" r:id="rId10"/>
     <sheet name="Search Order By Name" sheetId="11" r:id="rId11"/>
-    <sheet name="Search Order By Number" sheetId="12" r:id="rId12"/>
-    <sheet name="Select Order" sheetId="13" r:id="rId13"/>
-    <sheet name="Search Order Tab" sheetId="14" r:id="rId14"/>
-    <sheet name="Close App" sheetId="15" r:id="rId15"/>
+    <sheet name="Select Order" sheetId="12" r:id="rId12"/>
+    <sheet name="Search Order Tab" sheetId="13" r:id="rId13"/>
+    <sheet name="Close App" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -614,25 +613,6 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>

</xml_diff>